<commit_message>
Added several routes for games and matches
Routes for adding matches to games have been added. The list with server routes is also updated.
</commit_message>
<xml_diff>
--- a/ServerRoutes.xlsx
+++ b/ServerRoutes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58">
   <si>
     <t>Route</t>
   </si>
@@ -88,10 +88,16 @@
     <t>Remove the competitions in the body of the request</t>
   </si>
   <si>
-    <t>/game/addMatches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adds the matches which will be followed throughout the game. </t>
+    <t>/game/addMatchesWithId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adds the matches which will be followed throughout the game via ID. The user chooses form a list. </t>
+  </si>
+  <si>
+    <t>/game/addMatchesWithCompetition</t>
+  </si>
+  <si>
+    <t>Adds all matches for a competition, which is included in the game.</t>
   </si>
   <si>
     <t>/game/getAll</t>
@@ -189,12 +195,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,37 +218,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -254,8 +239,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -263,53 +287,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,9 +309,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -348,7 +332,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -371,31 +370,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,19 +532,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,127 +544,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,36 +564,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -617,9 +590,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -629,6 +604,45 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,166 +661,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1132,10 +1131,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1305,7 +1304,7 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1319,7 +1318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1329,34 +1328,40 @@
       <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" ht="18.75" spans="1:1">
-      <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>42</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" ht="18.75" spans="1:1">
+      <c r="A24" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1378,23 +1383,23 @@
         <v>47</v>
       </c>
       <c r="C26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" ht="18.75" spans="1:1">
-      <c r="A28" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="29" ht="18.75" spans="1:1">
+      <c r="A29" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1419,9 +1424,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="3:3">
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>